<commit_message>
Updates to PCT Code Changes
</commit_message>
<xml_diff>
--- a/MVI_Sample_Prep_Helper_Template.xlsx
+++ b/MVI_Sample_Prep_Helper_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sys_op\methods\Development\AMEX_Template_BD\MVI_Sample_Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D83D4CD-3B5F-44B1-9F8B-9FD4BE65269C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5F78F6-04E3-434C-9ADE-FF0236393D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVI_Sample" sheetId="11" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="CV_Reporting_Names" sheetId="10" r:id="rId5"/>
     <sheet name="CV_Product_Codes" sheetId="6" r:id="rId6"/>
     <sheet name="Weighting_Segments" sheetId="9" r:id="rId7"/>
+    <sheet name="PCT_Code_Changes" sheetId="13" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_AMO_ContentDefinition_638163707" hidden="1">"'Partitions:13'"</definedName>
@@ -75,7 +76,7 @@
     <definedName name="_AMO_XmlVersion" hidden="1">"'1'"</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MVI_Sample!$B$1:$AG$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -454,7 +455,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="807">
   <si>
     <t>Country</t>
   </si>
@@ -2868,6 +2869,15 @@
   </si>
   <si>
     <t>ICC - IECC</t>
+  </si>
+  <si>
+    <t>Update_NA_Cell</t>
+  </si>
+  <si>
+    <t>Update_Product</t>
+  </si>
+  <si>
+    <t>Update_PCT_Code</t>
   </si>
 </sst>
 </file>
@@ -45004,7 +45014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -45012,7 +45022,7 @@
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" customWidth="1"/>
@@ -45414,7 +45424,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="63">
         <v>18</v>
       </c>
@@ -55545,6 +55555,61 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41731C0D-7C85-4CD0-AAB2-C08CD9D76422}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="96" t="s">
+        <v>804</v>
+      </c>
+      <c r="H1" s="96" t="s">
+        <v>805</v>
+      </c>
+      <c r="I1" s="96" t="s">
+        <v>806</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{4bba711e-105b-499f-91fa-eabdf1048d84}" enabled="1" method="Standard" siteId="{9cc6d92e-03c1-419b-9eec-0e7716a56d02}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Update PCT Code Changes sheet in template
</commit_message>
<xml_diff>
--- a/MVI_Sample_Prep_Helper_Template.xlsx
+++ b/MVI_Sample_Prep_Helper_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sys_op\methods\Development\AMEX_Template_BD\MVI_Sample_Prep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Development\AMEX_Sample_Prep_Templates\MVI_Sample_Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D34A744-530F-43B8-B33A-02299CC2FBDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1DC309-66CD-4CE2-B8B3-AA8B88BA10D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="2475" windowWidth="21600" windowHeight="11295" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVI_Sample" sheetId="11" r:id="rId1"/>
@@ -455,7 +455,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="696">
   <si>
     <t>Country</t>
   </si>
@@ -2529,16 +2529,22 @@
     <t>ICC - IECC</t>
   </si>
   <si>
-    <t>Update_Product</t>
-  </si>
-  <si>
-    <t>Update_PCT_Code</t>
-  </si>
-  <si>
-    <t>NA_Cell_Number</t>
-  </si>
-  <si>
-    <t>Update_NA_Cell_Number</t>
+    <t>Updated_NA_Cell_Number</t>
+  </si>
+  <si>
+    <t>Updated_PCT_Code</t>
+  </si>
+  <si>
+    <t>Updated_NA_Product_Code</t>
+  </si>
+  <si>
+    <t>Updated_Card_Product</t>
+  </si>
+  <si>
+    <t>Card_ProductAIF</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -51698,47 +51704,57 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41731C0D-7C85-4CD0-AAB2-C08CD9D76422}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>692</v>
+        <v>164</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>24</v>
       </c>
       <c r="D1" s="95" t="s">
         <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="F1" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="96" t="s">
+      <c r="G1" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="H1" s="96" t="s">
+        <v>690</v>
+      </c>
+      <c r="I1" s="96" t="s">
+        <v>692</v>
+      </c>
+      <c r="J1" s="96" t="s">
         <v>693</v>
       </c>
-      <c r="G1" s="96" t="s">
-        <v>690</v>
-      </c>
-      <c r="H1" s="96" t="s">
+      <c r="K1" s="96" t="s">
         <v>691</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add troubleshooting notes to documentation
</commit_message>
<xml_diff>
--- a/MVI_Sample_Prep_Helper_Template.xlsx
+++ b/MVI_Sample_Prep_Helper_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Development\AMEX_Sample_Prep_Templates\MVI_Sample_Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1DC309-66CD-4CE2-B8B3-AA8B88BA10D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE4C41A-A15E-4669-99AB-19A3413FBD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVI_Sample" sheetId="11" r:id="rId1"/>
@@ -368,6 +368,54 @@
     fields for Qualtric. Note that their placement in the PML file my have moved</t>
       </text>
     </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{E1778E21-B319-49C8-A4AF-5B8FAAF0CCCB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Beck DeYoung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+All of these should be "Y" or "N". If you see something like "Optional" for a cell in Germany. Change it in the MVI_Sample sheet to "Y".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{EFE3F6D2-CF4F-44E1-9226-60B105BE06A6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Beck DeYoung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+All of these should be numeric. If there are two cellsi in Thailand with values of 0, that is okay. If there are two cells in Thailand with non-numeric values, that is not okay. Go to the MVI_Sample sheet and find the two blacked out rows in Thailand and delete the values in the cells</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -375,10 +423,10 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Kim Hamilton</author>
+    <author>Beck DeYoung</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D7B45AED-BE88-4A27-8AF6-C37063A45880}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1DE6C94B-A059-41BE-BCE6-CD42521D5290}">
       <text>
         <r>
           <rPr>
@@ -386,20 +434,87 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Kim Hamilton:</t>
+          <t>Beck DeYoung:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Product code is unique to MVI &amp; not
- part of CMS system</t>
+DO NOT OVERRIDE THESE HEADERS. Just copy and paste everything below from the reporting names sheet</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Beck DeYoung</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CE1D41FC-5F5F-4F9C-BF32-1B243A77302E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Beck DeYoung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DO NOT OVERRIDE THESE HEADERS</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Beck DeYoung</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{EBEB83D8-1B37-4D24-A59B-95DE8E1AD4BB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Beck DeYoung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DO NOT OVERRIDE THESE HEADERS</t>
         </r>
       </text>
     </comment>
@@ -3590,7 +3705,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23659,8 +23774,8 @@
   <dimension ref="A1:Z294"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+      <pane xSplit="7" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45977,8 +46092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779C8E77-7838-49B0-90CD-566E292DFAD9}">
   <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="F250" sqref="F250"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48364,11 +48479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E78068-6155-4AF2-B347-6F45FDEA64C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E78068-6155-4AF2-B347-6F45FDEA64C3}">
   <dimension ref="A1:AD346"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51654,18 +51769,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FFBBD8-BB0F-4B28-A3B7-FA3AB08CD25F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FFBBD8-BB0F-4B28-A3B7-FA3AB08CD25F}">
   <sheetPr>
     <tabColor theme="3" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51699,6 +51815,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -51706,7 +51823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41731C0D-7C85-4CD0-AAB2-C08CD9D76422}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>